<commit_message>
Update planning for Governors
</commit_message>
<xml_diff>
--- a/文档/总督.xlsx
+++ b/文档/总督.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735F85F6-6CFB-4A46-9C73-E6BDECB170D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAED92B8-E42F-44D9-AFE8-3D6E97E5C2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="1425" windowWidth="29475" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="25200" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="132">
   <si>
     <t>瑞娜</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,10 +98,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>富贵安乐</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>本地线人</t>
   </si>
   <si>
@@ -255,6 +251,313 @@
   </si>
   <si>
     <t>扩核推手</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>绰有余裕</t>
+  </si>
+  <si>
+    <t>加速城市获得单元格的速度。每个通过本城的国际贸易路线提供3金币</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>港口和商业中心相邻加成翻倍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有（离岸）风电农场、太阳能农场、地热发电厂和水电站坝提供+2电力、+2金币</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>允许城市使用金币购买区域</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个公民+2金币</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个未改良地貌+2金币。与未改良地貌相邻的单元格获得+1魅力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上任只需3回合。增强城市驻军战斗力5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>城市领土内的单位在防御时+5战斗力，9格内的城市+4忠诚度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>城市无法被围攻。战略资源每回合额外获得1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>城市可以进行两次远程攻击。本城训练单位获得一个免费的初始升级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城领土内的防空单位+25防空战斗力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有核武项目+30%生产力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可被派驻至城邦，视作2使者</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9格内的外国城市-2忠诚度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得城邦的奢侈资源1份</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城的敌方间谍下降3级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得城邦的战略资源，若为宗主则翻倍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>翻倍本城邦的使者数目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收获单元格资源和移除地貌的产出+50%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>余粮+20%。以此为终点的贸易路线向发起城市提供+2粮食</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城建造移民不消耗人口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>煤电站、油电站和核电站每份资源产生的电力+1，生产力+2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生产单位所需的战略资源-80%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城获得6格内所有工业区的产能加成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城宗教压力翻倍，每个城区提供+2信仰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城宗教单位+10宗教战斗力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城所有单位一回合可回满生命值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城不受其他玩家宗教的压力和战斗效果影响。完成建筑建设时获得25%信仰返利</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使徒与武僧在获得第一次升级时额外获得一次升级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>允许使用信仰购买区域</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城建造的建造者+1建造次数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城建设区域+20%生产力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>允许建造渔场改良设施（+1粮、相邻一个海洋资源+1粮，+0.5住房、梁总督存在时+1生产力）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城的改良、建筑和区域不受环境效果伤害</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个社区和水渠+2住房，每个运河和堤坝+1宜居</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>允许建造城市公园改良设施（相邻单元格+2魅力，+1文化，沿水+1宜居，梁总督存在时+3文化）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城+15%瓶琴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城伟人点数+100%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城美术、音乐、文学巨作的旅游业绩+100%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城太空计划项目+30%生产力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个公民+1文化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个公民+1科技</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原版（风云变幻）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改草案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城剧院广场相邻加成翻倍，露天剧场和博物馆+25%文化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城学院相邻加成翻倍，图书馆和公立学校+25%科技</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>允许建造渔场改良设施（+2粮、相邻一个海洋资源+1粮，+0.5住房、梁总督存在时+2生产力）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>允许建造城市公园改良设施（相邻单元格+2魅力，+3文化，沿水+1宜居，梁总督存在时+3文化）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城建设区域和建筑+30%生产力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不做改动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>准备修改</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城所有单位驻扎一回合可回满生命值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>资源管理、产能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>信仰、宗教力量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>建筑、改良设施</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>科技、文化、伟人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使者、城邦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>军事、防御</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金币、财政</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生产单位所需的战略资源-50%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9格内的外国城市-4忠诚度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上任只需3回合。增强城市防御战斗力5，9格内的城市+4忠诚度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>城市领土内的单位在防御时+5战斗力，本城训练单位获得一个免费的初始升级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>城市无法被围攻。战略资源每回合额外获得1，战略资源+1生产力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城建造移民不消耗人口。以此为终点的贸易路线向发起城市提供+1生产力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>余粮+20%。以此为终点的贸易路线向发起城市提供+1粮食</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个公民+2金币，完成建筑建设时获得25%金币返利</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有（离岸）风电农场、太阳能农场、地热发电厂和水电站坝提供+2电力、+2金币；本城沿河地块+2金币，地热裂缝+4金币</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>扩军推手</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城训练军事单位和进行所有核武项目+30%生产力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个未改良地貌+4金币。与未改良地貌相邻的单元格获得+1魅力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>城市可以进行两次远程攻击，且远程攻击力+5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水渠和堤坝+2宜居度，+2住房</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>煤电站、油电站和核电站每份资源产生的电力+2。每个工业区建筑生产力+2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>港口和商业中心相邻加成翻倍。每个通过本城的国际贸易路线提供3金币</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加速城市获得单元格的速度。本城购买单元格所需的费用-20%。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -285,12 +588,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -307,7 +622,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -319,6 +634,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -595,244 +928,731 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="5" width="9" style="1"/>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="19.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="1"/>
+    <col min="4" max="4" width="21" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1"/>
     <col min="6" max="6" width="14.125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="7" max="7" width="9" style="1"/>
+    <col min="8" max="8" width="19.875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="1"/>
+    <col min="10" max="10" width="18.875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="1"/>
+    <col min="12" max="12" width="22" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9" style="1"/>
+    <col min="14" max="14" width="23.375" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2" t="s">
+    <row r="3" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="3"/>
+      <c r="H3" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="I3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3" t="s">
+      <c r="J3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="2" t="s">
+      <c r="L5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="N3" s="3"/>
+      <c r="N5" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+    <row r="6" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A10" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A12" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="N12" s="5"/>
+    </row>
+    <row r="13" spans="1:16" ht="54" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="P13" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="54" x14ac:dyDescent="0.15">
+      <c r="A14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="54" x14ac:dyDescent="0.15">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="54" x14ac:dyDescent="0.15">
+      <c r="A16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="2" t="s">
+      <c r="D16" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
+      <c r="F16" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
+      <c r="H16" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="2" t="s">
+      <c r="J16" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="K16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" s="3"/>
+      <c r="L16" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
+    <row r="17" spans="1:14" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
+      <c r="B17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="2" t="s">
+      <c r="F17" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
+      <c r="H17" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="2" t="s">
+      <c r="J17" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="N5" s="3"/>
+      <c r="L17" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="2" t="s">
+    <row r="18" spans="1:14" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="A18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
+      <c r="F18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="2" t="s">
+      <c r="H18" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3" t="s">
+      <c r="L18" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="M18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="N7" s="3"/>
+      <c r="N18" s="7" t="s">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A10:N10"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Prep for Governors overhaul
</commit_message>
<xml_diff>
--- a/文档/总督.xlsx
+++ b/文档/总督.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAED92B8-E42F-44D9-AFE8-3D6E97E5C2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB2F2E6-7E63-46BA-9CA1-182CE0E523D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="25200" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="137">
   <si>
     <t>瑞娜</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -513,14 +513,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>本城建造移民不消耗人口。以此为终点的贸易路线向发起城市提供+1生产力</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>余粮+20%。以此为终点的贸易路线向发起城市提供+1粮食</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>每个公民+2金币，完成建筑建设时获得25%金币返利</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -533,14 +525,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>本城训练军事单位和进行所有核武项目+30%生产力</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>每个未改良地貌+4金币。与未改良地貌相邻的单元格获得+1魅力</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>城市可以进行两次远程攻击，且远程攻击力+5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -557,7 +541,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>加速城市获得单元格的速度。本城购买单元格所需的费用-20%。</t>
+    <t>本城购买单元格所需的费用-20%。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>森林、雨林和沼泽+2金币。与未改良地貌相邻的单元格获得+1魅力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以此为终点的贸易路线向发起城市提供+1粮食+1生产力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城建造移民不消耗人口。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城建造项目+30%生产力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城训练军事单位+30%生产力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本城领土内的防空单位+25防空战斗力，军事单位防御空中单位+15战斗力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防空计划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>绰有余裕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>规划专员</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -638,12 +658,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -652,6 +666,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -930,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -954,22 +974,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
     </row>
     <row r="2" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -1280,22 +1300,22 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
@@ -1342,41 +1362,41 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
+      <c r="D12" s="8"/>
+      <c r="E12" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5" t="s">
+      <c r="F12" s="8"/>
+      <c r="G12" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5" t="s">
+      <c r="H12" s="8"/>
+      <c r="I12" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5" t="s">
+      <c r="J12" s="8"/>
+      <c r="K12" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5" t="s">
+      <c r="L12" s="8"/>
+      <c r="M12" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="N12" s="5"/>
+      <c r="N12" s="8"/>
     </row>
-    <row r="13" spans="1:16" ht="54" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>36</v>
@@ -1387,34 +1407,34 @@
       <c r="E13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="5" t="s">
         <v>68</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="5" t="s">
         <v>74</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="J13" s="5" t="s">
         <v>80</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L13" s="7" t="s">
+      <c r="L13" s="5" t="s">
         <v>86</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="N13" s="7" t="s">
+      <c r="N13" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="P13" s="9" t="s">
+      <c r="P13" s="7" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1423,7 +1443,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>25</v>
@@ -1441,16 +1461,16 @@
         <v>20</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="J14" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>40</v>
+      <c r="K14" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>104</v>
@@ -1461,7 +1481,7 @@
       <c r="N14" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="P14" s="8" t="s">
+      <c r="P14" s="6" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1470,7 +1490,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>26</v>
@@ -1479,21 +1499,21 @@
         <v>119</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>70</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="J15" s="5" t="s">
         <v>107</v>
       </c>
       <c r="K15" s="2" t="s">
@@ -1514,62 +1534,62 @@
         <v>47</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="5" t="s">
         <v>71</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="7" t="s">
+      <c r="J16" s="5" t="s">
         <v>83</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L16" s="7" t="s">
+      <c r="L16" s="5" t="s">
         <v>89</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N16" s="7" t="s">
+      <c r="N16" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:14" ht="54" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>66</v>
+        <v>134</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="5" t="s">
         <v>72</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -1581,20 +1601,20 @@
       <c r="I17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="7" t="s">
+      <c r="J17" s="5" t="s">
         <v>84</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>43</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="M17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="N17" s="7" t="s">
-        <v>95</v>
+      <c r="N17" s="4" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="94.5" x14ac:dyDescent="0.15">
@@ -1602,30 +1622,30 @@
         <v>31</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="5" t="s">
         <v>73</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H18" s="5" t="s">
         <v>79</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J18" s="7" t="s">
+      <c r="J18" s="5" t="s">
         <v>85</v>
       </c>
       <c r="K18" s="2" t="s">
@@ -1637,7 +1657,7 @@
       <c r="M18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N18" s="7" t="s">
+      <c r="N18" s="5" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Buff Governors and Golden Age bonuses
</commit_message>
<xml_diff>
--- a/文档/总督.xlsx
+++ b/文档/总督.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7880F5A6-06D8-48B9-A696-BA61100B2579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2464AE8-CEC2-4AD8-9608-9E4718DCE598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10635" yWindow="1050" windowWidth="27915" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9855" yWindow="2655" windowWidth="27915" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="142">
   <si>
     <t>瑞娜</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -497,14 +497,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>9格内的外国城市-4忠诚度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上任只需3回合。增强城市防御战斗力5，9格内的城市+4忠诚度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>城市领土内的单位在防御时+5战斗力，本城训练单位获得一个免费的初始升级</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -537,10 +529,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>以此为终点的贸易路线向发起城市提供+1粮食+1生产力</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>本城建造移民不消耗人口。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -582,6 +570,120 @@
   </si>
   <si>
     <t>所有（离岸）风电农场、太阳能农场、地热发电厂提供+2电力、+2金币；水力发电坝提供+2电力；本城6格内有水力发电坝的沿河地块+2金币</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个公民+0.5瓶琴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>以此为终点的贸易路线向发起城市提供</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+2粮食+2生产力</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>本城宗教压力翻倍，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>每个公民+1信仰</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>收获单元格资源和移除地貌的产出+50%。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+50%余粮。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9格内的外国城市-8忠诚度。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>可被派驻至城邦，视作</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>使者</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>上任只需3回合。增强城市防御战斗力5，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>9格内的城市+4忠诚度，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>本城+20忠诚度</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -589,7 +691,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -606,6 +708,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -672,9 +789,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -686,7 +800,10 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -972,8 +1089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1413,50 +1530,50 @@
       </c>
       <c r="N12" s="10"/>
     </row>
-    <row r="13" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" ht="54" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>125</v>
+      <c r="B13" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>117</v>
+      <c r="D13" s="8" t="s">
+        <v>141</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>68</v>
+      <c r="F13" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>74</v>
+      <c r="H13" s="8" t="s">
+        <v>138</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="4" t="s">
-        <v>80</v>
+      <c r="J13" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L13" s="2" t="s">
         <v>86</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="N13" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="P13" s="6" t="s">
+      <c r="N13" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="P13" s="5" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1464,46 +1581,46 @@
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>124</v>
+      <c r="B14" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>118</v>
+      <c r="D14" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>126</v>
+      <c r="H14" s="8" t="s">
+        <v>136</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="2" t="s">
         <v>81</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="L14" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>104</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="N14" s="9" t="s">
+      <c r="N14" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="P14" s="5" t="s">
+      <c r="P14" s="4" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1511,181 +1628,181 @@
       <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>134</v>
+      <c r="B15" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>119</v>
+      <c r="D15" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F15" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>127</v>
+      <c r="H15" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" s="2" t="s">
         <v>107</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L15" s="9" t="s">
+      <c r="L15" s="2" t="s">
         <v>102</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="N15" s="9" t="s">
+      <c r="N15" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="P15" s="7" t="s">
-        <v>132</v>
+      <c r="P15" s="6" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="54" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>121</v>
+      <c r="D16" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="2" t="s">
         <v>71</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="9" t="s">
-        <v>123</v>
+      <c r="H16" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="2" t="s">
         <v>83</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="L16" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N16" s="4" t="s">
+      <c r="N16" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="P16" s="8" t="s">
-        <v>133</v>
+      <c r="P16" s="7" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="54" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>136</v>
+        <v>126</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="9" t="s">
+      <c r="H17" s="2" t="s">
         <v>115</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="2" t="s">
         <v>84</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="L17" s="9" t="s">
-        <v>122</v>
+      <c r="L17" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="M17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="N17" s="9" t="s">
-        <v>128</v>
+      <c r="N17" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>137</v>
+      <c r="B18" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>135</v>
+        <v>118</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="2" t="s">
         <v>79</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="2" t="s">
         <v>85</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L18" s="9" t="s">
+      <c r="L18" s="2" t="s">
         <v>103</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N18" s="4" t="s">
+      <c r="N18" s="2" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>